<commit_message>
sep update + mpi and changes to social benefits and taxes
</commit_message>
<xml_diff>
--- a/results/10-2022/comparison-deflators-10-2022.xlsx
+++ b/results/10-2022/comparison-deflators-10-2022.xlsx
@@ -831,31 +831,31 @@
         <v>-0.0866</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.0189</v>
+        <v>-0.0165</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0137</v>
+        <v>-0.0037</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1496</v>
+        <v>0.1672</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0511</v>
+        <v>0.0786</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0041</v>
+        <v>0.0371</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.048</v>
+        <v>-0.0128</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0918</v>
+        <v>-0.0628</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0071</v>
+        <v>0.0278</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0191</v>
+        <v>0.0256</v>
       </c>
     </row>
     <row r="8">
@@ -884,31 +884,31 @@
         <v>-0.6023</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.4293</v>
+        <v>-0.4514</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.2972</v>
+        <v>-0.2684</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.2003</v>
+        <v>-0.1513</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.1331</v>
+        <v>-0.0996</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.0215</v>
+        <v>-0.0022</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2833</v>
+        <v>0.2975</v>
       </c>
       <c r="O8" t="n">
-        <v>0.2871</v>
+        <v>0.3056</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3106</v>
+        <v>0.3289</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2942</v>
+        <v>0.3225</v>
       </c>
     </row>
     <row r="9">
@@ -1096,31 +1096,31 @@
         <v>-0.8555</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.8122</v>
+        <v>-0.5935</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.3733</v>
+        <v>-0.1412</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.2418</v>
+        <v>-0.015</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.1678</v>
+        <v>0.0539</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0535</v>
+        <v>-0.0446</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0508</v>
+        <v>-0.0601</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0487</v>
+        <v>-0.0578</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0467</v>
+        <v>-0.0556</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0264</v>
+        <v>-0.0351</v>
       </c>
     </row>
     <row r="13">
@@ -1308,31 +1308,31 @@
         <v>-2.8519</v>
       </c>
       <c r="I16" t="n">
-        <v>-2.1288</v>
+        <v>-1.9323</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.9507</v>
+        <v>-1.6849</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.6888</v>
+        <v>-2.403</v>
       </c>
       <c r="L16" t="n">
-        <v>-1.133</v>
+        <v>-0.8625</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.4886</v>
+        <v>-0.4285</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.1933</v>
+        <v>-0.1597</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.3996</v>
+        <v>-0.3649</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.4059</v>
+        <v>-0.3748</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.0801</v>
+        <v>-0.0532</v>
       </c>
     </row>
     <row r="17">
@@ -1732,31 +1732,31 @@
         <v>-0.0957</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.0134</v>
+        <v>-0.0159</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0794</v>
+        <v>0.0745</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0021</v>
+        <v>-0.0054</v>
       </c>
       <c r="L24" t="n">
-        <v>0.186</v>
+        <v>0.1739</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1514</v>
+        <v>0.1421</v>
       </c>
       <c r="N24" t="n">
-        <v>0.1252</v>
+        <v>0.1185</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0992</v>
+        <v>0.0954</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.0677</v>
+        <v>-0.0667</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.0545</v>
+        <v>-0.0538</v>
       </c>
     </row>
     <row r="25">
@@ -2315,31 +2315,31 @@
         <v>0.0045</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0047</v>
+        <v>0.0071</v>
       </c>
       <c r="J35" t="n">
+        <v>0.0148</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.0227</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.0295</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.0424</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.0357</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.0187</v>
+      </c>
+      <c r="Q35" t="n">
         <v>0.0048</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.0051</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0.0021</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0.0012</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="O35" t="n">
-        <v>-0.0002</v>
-      </c>
-      <c r="P35" t="n">
-        <v>-0.002</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>-0.0017</v>
       </c>
     </row>
     <row r="36">
@@ -2368,31 +2368,31 @@
         <v>0.2658</v>
       </c>
       <c r="I36" t="n">
-        <v>0.2581</v>
+        <v>0.236</v>
       </c>
       <c r="J36" t="n">
-        <v>0.123</v>
+        <v>0.1518</v>
       </c>
       <c r="K36" t="n">
-        <v>0.1204</v>
+        <v>0.1694</v>
       </c>
       <c r="L36" t="n">
-        <v>0.1179</v>
+        <v>0.1514</v>
       </c>
       <c r="M36" t="n">
-        <v>0.1154</v>
+        <v>0.1347</v>
       </c>
       <c r="N36" t="n">
-        <v>0.1133</v>
+        <v>0.1275</v>
       </c>
       <c r="O36" t="n">
-        <v>0.1111</v>
+        <v>0.1296</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.0121</v>
+        <v>0.0063</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.0115</v>
+        <v>0.0168</v>
       </c>
     </row>
     <row r="37">
@@ -2580,31 +2580,31 @@
         <v>0.1483</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.0335</v>
+        <v>0.1852</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.0328</v>
+        <v>0.1992</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.0322</v>
+        <v>0.1946</v>
       </c>
       <c r="L40" t="n">
-        <v>-0.1718</v>
+        <v>0.0499</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0002</v>
+        <v>0.0092</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0004</v>
+        <v>-0.0089</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0004</v>
+        <v>-0.0087</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0004</v>
+        <v>-0.0085</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.0004</v>
+        <v>-0.0083</v>
       </c>
     </row>
     <row r="41">
@@ -2792,31 +2792,31 @@
         <v>0.5796</v>
       </c>
       <c r="I44" t="n">
-        <v>0.2017</v>
+        <v>0.3982</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0594</v>
+        <v>0.3253</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0766</v>
+        <v>0.3624</v>
       </c>
       <c r="L44" t="n">
-        <v>-0.0305</v>
+        <v>0.2401</v>
       </c>
       <c r="M44" t="n">
-        <v>0.1427</v>
+        <v>0.2028</v>
       </c>
       <c r="N44" t="n">
-        <v>0.1409</v>
+        <v>0.1745</v>
       </c>
       <c r="O44" t="n">
-        <v>0.1386</v>
+        <v>0.1732</v>
       </c>
       <c r="P44" t="n">
-        <v>-0.0328</v>
+        <v>-0.0016</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.0095</v>
+        <v>0.0174</v>
       </c>
     </row>
     <row r="45">
@@ -3216,31 +3216,31 @@
         <v>-0.0368</v>
       </c>
       <c r="I52" t="n">
-        <v>-0.0366</v>
+        <v>-0.0391</v>
       </c>
       <c r="J52" t="n">
-        <v>-0.0364</v>
+        <v>-0.0414</v>
       </c>
       <c r="K52" t="n">
-        <v>-0.0364</v>
+        <v>-0.0439</v>
       </c>
       <c r="L52" t="n">
-        <v>-0.0026</v>
+        <v>-0.0147</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.0016</v>
+        <v>-0.011</v>
       </c>
       <c r="N52" t="n">
-        <v>-0.0007</v>
+        <v>-0.0073</v>
       </c>
       <c r="O52" t="n">
-        <v>0.0003</v>
+        <v>-0.0036</v>
       </c>
       <c r="P52" t="n">
-        <v>0.0023</v>
+        <v>0.0032</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.0021</v>
+        <v>0.0029</v>
       </c>
     </row>
     <row r="53">

</xml_diff>